<commit_message>
next step to do.
</commit_message>
<xml_diff>
--- a/document/工作计划.xlsx
+++ b/document/工作计划.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ADC7C324-CF9C-4BC7-AAA8-CBB76D6D6E7C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{844C6120-13C7-4969-B431-5AB2839BC50D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>下一步任务</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,8 +45,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>主页、评论页面、购物车js的编写
-主页、评论页面、购物车用jsp写</t>
+    <t>js编写完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">主页、评论页面、购物车js的编写
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评论信息列表类
+商品信息类
+购物车商品信息类
+主页、评论页面、购物车用jsp写
+实现交互</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -97,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -111,6 +123,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,9 +443,11 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -440,7 +457,9 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>

</xml_diff>